<commit_message>
Changed and updated the parts list
</commit_message>
<xml_diff>
--- a/OrbitalShaker_ElectronicsPartsList.xlsx
+++ b/OrbitalShaker_ElectronicsPartsList.xlsx
@@ -8,8 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Components" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Fixings &amp; Tools" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Electronics Parts" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Laboratory Parts" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Fixings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="LED Illuminator Parts" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Tools" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -431,16 +434,85 @@
     <t xml:space="preserve">SPC15494</t>
   </si>
   <si>
-    <t xml:space="preserve">40mm Fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 VDC Fan, 60mA, 40mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2816685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC002106</t>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orbital Shaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eBay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">283712826465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KJ-201BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 nut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 zinc-plated steel nut (pack of 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR Fastenings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1419449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4-HFST-Z100-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 zinc-plated steel washer (pack of 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2506009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM4-FASTWAZ100DIN125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4×12 screw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 12mm zinc-plated pan head screw (pack of 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1419994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 12 PRSTMC Z100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3×10 screw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 10mm countersunk zinc-plated screw (pack of 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1420398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 10 KRSTMC Z100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50mm M4 Standoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50mm M4 standoff male-female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ettinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1466738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05.14.501</t>
   </si>
   <si>
     <t xml:space="preserve">1m LED Strip</t>
@@ -470,91 +542,22 @@
     <t xml:space="preserve">15DYS624-300100W-K</t>
   </si>
   <si>
-    <t xml:space="preserve">50mm M4 Standoff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50mm M4 standoff male-female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ettinger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1466738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05.14.501</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 nut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 zinc-plated steel nut (pack of 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR Fastenings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1419449</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4-HFST-Z100-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 washer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 zinc-plated steel washer (pack of 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2506009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM4-FASTWAZ100DIN125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4×12 screw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 12mm zinc-plated pan head screw (pack of 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1419994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 12 PRSTMC Z100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3×10 screw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 10mm countersunk zinc-plated screw (pack of 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1420398</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 10 KRSTMC Z100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 tap set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 thread tap set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">375238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230-030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black cable</t>
+    <t xml:space="preserve">LED Heatsink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heatsink, 200 mm x 150 mm x 40 mm, 0.5 °C/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fischer Elektronik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4621906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK 47/150 SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Cable</t>
   </si>
   <si>
     <r>
@@ -596,7 +599,7 @@
     <t xml:space="preserve">PP001185</t>
   </si>
   <si>
-    <t xml:space="preserve">red cable</t>
+    <t xml:space="preserve">Red Cable</t>
   </si>
   <si>
     <r>
@@ -634,6 +637,319 @@
   <si>
     <t xml:space="preserve">PP001269</t>
   </si>
+  <si>
+    <t xml:space="preserve">Clear Acrylic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 mm clear acrylic sheet (any make, &gt; 30 cm × 20 cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">824-660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24H Time Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmable 24-hour socket time switch (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2777066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEL00407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workshop Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 Tap Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 thread tap set (any make, #4-40 for imperial threads)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">375238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230-030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap Wrench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap Wrench (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">241 001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tool Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mechanical workshop tool kit (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">829-6561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General digital multimeter (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123-1930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stationeries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multipurpose Glue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All purpose clear adhesive (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bostik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0001OZI48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrical Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PVC Electrical Insulation tape (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PVC TAPE 1920B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scissors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common scissors (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B00XP1V0UU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford 13cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine tip permanent marker pen (not black, any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staedtler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B005DPPQAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruler 30 cm (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q Connect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B000NMBTUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tweezers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Watchmakers tweezers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (any make)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Duratool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3127692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1PK-125T-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder flux (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip Quik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1850220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD291NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin solder wire (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3262209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D03341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering Station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering station suitable for SMD (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metcal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1560738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS-900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isopropyl alcohol for cleaning (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexeal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B079YVPZDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D Printer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FDM 3D Printer with build material (any make, or outsource)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratasys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uPrint SE Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cutting and Drilling Tools (Either tools or laser cutter, both not required)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General hand or pillar drill (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B00IINANZ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6221AB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4mm Drill Bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSS drill bit 4 mm (any make, ideally spur-point bit for plastic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">378124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201 040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacksaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 mm hacksaw (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2103261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D02166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P150 Sandpaper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P80-P180 sandpaper (any make)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001PNBC0I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser Cutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional laser cutter for plastics (any make)</t>
+  </si>
 </sst>
 </file>
 
@@ -643,7 +959,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -685,6 +1001,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -729,7 +1050,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -754,8 +1075,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -766,8 +1095,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -787,10 +1144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1828,147 +2185,12 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="J31" s="1" t="n">
-        <f aca="false">I31*B31</f>
-        <v>7.92</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <f aca="false">1+A31</f>
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>9009079</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>25.84</v>
-      </c>
-      <c r="J32" s="1" t="n">
-        <f aca="false">I32*B32</f>
-        <v>51.68</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <f aca="false">1+A32</f>
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I33" s="1" t="n">
-        <v>23.37</v>
-      </c>
-      <c r="J33" s="1" t="n">
-        <f aca="false">I33*B33</f>
-        <v>23.37</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <f aca="false">1+A33</f>
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="J34" s="1" t="n">
-        <f aca="false">I34*B34</f>
-        <v>2.92</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J35" s="5" t="n">
-        <f aca="false">SUM(J2:J34)</f>
-        <v>124.34</v>
+      <c r="J31" s="5" t="n">
+        <f aca="false">SUM(J2:J30)</f>
+        <v>38.45</v>
       </c>
     </row>
   </sheetData>
@@ -2002,10 +2224,6 @@
     <hyperlink ref="G28" r:id="rId27" display="9473556"/>
     <hyperlink ref="G29" r:id="rId28" display="2854809"/>
     <hyperlink ref="G30" r:id="rId29" display="2668408"/>
-    <hyperlink ref="G31" r:id="rId30" display="2816685"/>
-    <hyperlink ref="G32" r:id="rId31" display="2214009"/>
-    <hyperlink ref="G33" r:id="rId32" display="2771453"/>
-    <hyperlink ref="G34" r:id="rId33" display="1466738"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2022,18 +2240,118 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>95.3</v>
+      </c>
+    </row>
+    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="n">
+        <v>95.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="283712826465"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.22"/>
@@ -2081,22 +2399,22 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>1.59</v>
@@ -2108,25 +2426,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>1.14</v>
@@ -2141,22 +2459,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>2.08</v>
@@ -2171,22 +2489,22 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>1.64</v>
@@ -2198,104 +2516,41 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>8.77</v>
+        <v>0.73</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>8.77</v>
+        <f aca="false">I6*B6</f>
+        <v>2.92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I7" s="6" t="n">
-        <v>0.315</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>0.315</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <f aca="false">SUM(J2:J8)</f>
-        <v>16.48</v>
+      <c r="A7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <f aca="false">SUM(J2:J6)</f>
+        <v>9.37</v>
       </c>
     </row>
   </sheetData>
@@ -2304,9 +2559,1217 @@
     <hyperlink ref="G3" r:id="rId2" display="2506009"/>
     <hyperlink ref="G4" r:id="rId3" display="1419994"/>
     <hyperlink ref="G5" r:id="rId4" display="1420398"/>
-    <hyperlink ref="G6" r:id="rId5" display="375238"/>
-    <hyperlink ref="G7" r:id="rId6" display="2528081"/>
-    <hyperlink ref="G8" r:id="rId7" display="2528174"/>
+    <hyperlink ref="G6" r:id="rId5" display="1466738"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>9009079</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <f aca="false">I2*B2</f>
+        <v>51.68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <f aca="false">1+A2</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>23.37</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <f aca="false">I3*B3</f>
+        <v>23.37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <f aca="false">1+A3</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <f aca="false">I4*B4</f>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <f aca="false">1+A4</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>35.71</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <f aca="false">B5*I5</f>
+        <v>35.71</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <f aca="false">1+A5</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <f aca="false">B6*I6</f>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <f aca="false">1+A6</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <f aca="false">B7*I7</f>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <f aca="false">1+A7</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>32.72</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <f aca="false">B8*I8</f>
+        <v>32.72</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <f aca="false">1+A8</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <f aca="false">B9*I9</f>
+        <v>2.01</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5" t="n">
+        <f aca="false">SUM(J2:J9)</f>
+        <v>149.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="2214009"/>
+    <hyperlink ref="G3" r:id="rId2" display="2771453"/>
+    <hyperlink ref="G4" r:id="rId3" display="1466738"/>
+    <hyperlink ref="G5" r:id="rId4" display="4621906"/>
+    <hyperlink ref="G6" r:id="rId5" display="2528081"/>
+    <hyperlink ref="G7" r:id="rId6" display="2528174"/>
+    <hyperlink ref="G8" r:id="rId7" display="824-660"/>
+    <hyperlink ref="G9" r:id="rId8" display="2777066"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I3" s="16" t="n">
+        <v>8.77</v>
+      </c>
+      <c r="J3" s="17" t="n">
+        <f aca="false">I3*B3</f>
+        <v>8.77</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="n">
+        <f aca="false">1+A3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I4" s="16" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="J4" s="17" t="n">
+        <f aca="false">I4*B4</f>
+        <v>10.71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="n">
+        <f aca="false">1+A4</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I5" s="17" t="n">
+        <v>108.59</v>
+      </c>
+      <c r="J5" s="17" t="n">
+        <f aca="false">I5*B5</f>
+        <v>108.59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="n">
+        <f aca="false">1+A5</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="17" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" s="17" t="n">
+        <f aca="false">I6*B6</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="n">
+        <f aca="false">1+A6</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="I8" s="17" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="J8" s="17" t="n">
+        <f aca="false">I8*B8</f>
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="n">
+        <f aca="false">1+A8</f>
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9" s="17" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="J9" s="17" t="n">
+        <f aca="false">I9*B9</f>
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="n">
+        <f aca="false">1+A9</f>
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I10" s="17" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="J10" s="17" t="n">
+        <f aca="false">I10*B10</f>
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <f aca="false">1+A10</f>
+        <v>8</v>
+      </c>
+      <c r="B11" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <v>733449</v>
+      </c>
+      <c r="I11" s="17" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="J11" s="17" t="n">
+        <f aca="false">I11*B11</f>
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="n">
+        <f aca="false">1+A11</f>
+        <v>9</v>
+      </c>
+      <c r="B12" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="I12" s="17" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="J12" s="17" t="n">
+        <f aca="false">I12*B12</f>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <f aca="false">1+A12</f>
+        <v>10</v>
+      </c>
+      <c r="B14" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="I14" s="17" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="J14" s="17" t="n">
+        <f aca="false">I14*B14</f>
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <f aca="false">1+A14</f>
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="I15" s="17" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="J15" s="17" t="n">
+        <f aca="false">I15*B15</f>
+        <v>11.94</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="n">
+        <f aca="false">1+A15</f>
+        <v>12</v>
+      </c>
+      <c r="B16" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="I16" s="17" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="J16" s="17" t="n">
+        <f aca="false">I16*B16</f>
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
+        <f aca="false">1+A16</f>
+        <v>13</v>
+      </c>
+      <c r="B17" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="I17" s="17" t="n">
+        <v>187</v>
+      </c>
+      <c r="J17" s="17" t="n">
+        <f aca="false">I17*B17</f>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
+        <f aca="false">1+A17</f>
+        <v>14</v>
+      </c>
+      <c r="B18" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" s="17" t="n">
+        <v>6.79</v>
+      </c>
+      <c r="J18" s="17" t="n">
+        <f aca="false">I18*B18</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="n">
+        <f aca="false">1+A18</f>
+        <v>15</v>
+      </c>
+      <c r="B20" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="n">
+        <f aca="false">1+A20</f>
+        <v>16</v>
+      </c>
+      <c r="B22" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="I22" s="17" t="n">
+        <v>44.99</v>
+      </c>
+      <c r="J22" s="17" t="n">
+        <f aca="false">I22*B22</f>
+        <v>44.99</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <f aca="false">1+A22</f>
+        <v>17</v>
+      </c>
+      <c r="B23" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="I23" s="17" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="J23" s="17" t="n">
+        <f aca="false">I23*B23</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="n">
+        <f aca="false">1+A23</f>
+        <v>18</v>
+      </c>
+      <c r="B24" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="I24" s="17" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="J24" s="17" t="n">
+        <f aca="false">I24*B24</f>
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="n">
+        <f aca="false">1+A24</f>
+        <v>19</v>
+      </c>
+      <c r="B25" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="H25" s="11" t="n">
+        <v>20150</v>
+      </c>
+      <c r="I25" s="17" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="J25" s="17" t="n">
+        <f aca="false">I25*B25</f>
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="n">
+        <f aca="false">1+A25</f>
+        <v>20</v>
+      </c>
+      <c r="B26" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="5" t="n">
+        <f aca="false">SUM(J3:J26)</f>
+        <v>435.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A21:J21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" display="375238"/>
+    <hyperlink ref="G4" r:id="rId2" display="376395"/>
+    <hyperlink ref="G5" r:id="rId3" display="829-6561"/>
+    <hyperlink ref="G6" r:id="rId4" display="123-1930"/>
+    <hyperlink ref="G8" r:id="rId5" display="B0001OZI48"/>
+    <hyperlink ref="G9" r:id="rId6" display="152346"/>
+    <hyperlink ref="G10" r:id="rId7" display="B00XP1V0UU"/>
+    <hyperlink ref="G11" r:id="rId8" display="B005DPPQAG"/>
+    <hyperlink ref="G12" r:id="rId9" display="B000NMBTUK"/>
+    <hyperlink ref="G14" r:id="rId10" display="3127692"/>
+    <hyperlink ref="G15" r:id="rId11" display="1850220"/>
+    <hyperlink ref="G16" r:id="rId12" display="3262209"/>
+    <hyperlink ref="G17" r:id="rId13" display="1560738"/>
+    <hyperlink ref="G18" r:id="rId14" display="B079YVPZDF"/>
+    <hyperlink ref="G20" r:id="rId15" display="uPrint SE Plus"/>
+    <hyperlink ref="G22" r:id="rId16" display="B00IINANZ8"/>
+    <hyperlink ref="G23" r:id="rId17" display="378124"/>
+    <hyperlink ref="G24" r:id="rId18" display="2103261"/>
+    <hyperlink ref="G25" r:id="rId19" display="B001PNBC0I"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>